<commit_message>
first draft of all 4 plotly charts
</commit_message>
<xml_diff>
--- a/DATA/books.xlsx
+++ b/DATA/books.xlsx
@@ -27,366 +27,6 @@
     <t xml:space="preserve">[screenplay] </t>
   </si>
   <si>
-    <t xml:space="preserve"> “Lives of the Monster Dogs” -Kirsten Bakis </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Martian Time-Slip" -Philip K. Dick </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Lullaby" -Jonathan Maberry </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Elevation" &amp; "Laurie" -Stephen King </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Switch House" -Tim Meyer </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Do Androids Dream of Electric Sheep" -Philip K. Dick </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Night" -Elie Wiesel </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Bumpy Night on the Walk of Fame" -Loretta Bolger Wish </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Most Dangerous Game" Richard Connell </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Cats of Cthulhu" -Chris W. Sears </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Tales of the Unusual" -Luke Smitherd </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Raiding Jotunheim- Valhalla Online, Book 2" -Kevin O. McLaughlin </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Valhalla Online" -Kevin O. McLaughlin </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Picture of Dorian Gray" -Oscar Wilde </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Born on a Blue Day" -Daniel Temmet </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Head On" -John Scalzi </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Lock In" -John Scalzi </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Space Opera" -Catherynne M. Valente </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Outsider" -Stephen King </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Neuromancer" -William Gibson </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "A Long December" -Richard Chizmar </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Moon is  Harsh Mistress" -Robert A. Heinlein </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Time for the Stars" -Robert A. Heinlein </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Man in the Empty Suit" -Sean Ferrell </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Man Who Folded Himself" -David Gerrold </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Artemis" -Andy Weir </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Martian" -Andy Weir </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Double Feature" -Owen King </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Widow's Point" -Richard Chizmar &amp; Billy Chizmar </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Sleeping Beauties" -Stephen King &amp; Owen King </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Wendigo" -author unknown- </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Secret of Chimneys" -Agatha Christie </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Greener Pastures" -Michael Wehunt </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Christmas Spirit" -Brian James Freeman </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Honey" -Sarah Sheldon </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Hex" -Thomas Olde Heuvelt </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Nine Billion Names of God" -Arthur D. Clarke </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Drawing Dead" -Brian McKinley </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Chthon" -Piers Anthony </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Outlander" -Diana Gabaldon </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Hitchhiker's Guide to the Galaxy" -Douglas Adams </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Gwendy's Button Box" -Stephen King &amp; Richard Chizmar </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Cemetery Dance, Issue #1" -various authors- </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Hero with a Thousand Faces" -Joseph Campbell </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Mr. Bubbles and the Mystery of the Mayan Temple" -Chris Sears </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Warlord of Mars" -Edgar Rice Burroughs </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Gods of Mars" -Edgar Rice Burroughs </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Wreck of the Titan" -Morgan Robertson </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "A Princess of Mars" -Edgar Rice Burroughs </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Consciousness Plague" -Paul Levinson </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Plot to Save Socrates" -Paul Levinson </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Urban Gothic" -Brian Keene </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Consultant" -Bentley Little </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Fireman" -Joe Hill </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Marvels" -Brian Selznik </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Charlie the Choo-Choo" -Stephen King </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Last Rung on the Ladder" -David Martin </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Interview with the Vampire" -Anne Rice </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Limetown" -Zack Akers </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Cemetery Dance, Issue #73" -various authors- </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Hallowe'en Party" -Agatha Christie </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Five Little Pigs" -Agatha Christie </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Save the Cat!" -Blake Snyder </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Brothers Karamazov" -Fyodor Dostoyevsky </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Eleven" -Patricia Reilly Giff </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "What Dreams May Come" -Richard Matheson </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Inferno" -Dan Brown </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Silver Scepter" -JD Mankowski </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Halloween Tree" -Ray Bradbury </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Halloween Man" -Douglas Clegg </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Haunted" -Bentley Little </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Thief of Always" -Clive Barker </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "20th Century Ghosts" -Joe Hill </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "End of Watch" -Stephen King </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Long Walk" -Stephen King </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Dispossessed" -Ursula K. Le Guin </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Dune" -Frank Herbert </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Armada" -Ernest Cline </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Patient Zero" -Jonathan Mayberry </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Son" -Lois Lowry </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Adventures of Sherlock Holmes" -Arthur Conan Doyle </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Speaking From Among the Bones" -Alan Bradley </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "City of Orphans" -Avi </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Hound of the Baskervilles" -Arthur Conan Doyle </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Physics of the Dead" -Luke Smitherd </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Inquisitor's Apprentice" -Chris Moriarty </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Foundation" -Isaac Asimov </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Red Moon" -Benjamin Percy </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Outview" -Brandt Legg </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "A Head Full of Knives" -Luke Smitherd </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "In the Darkness" -Luke Smitherd </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Weird, Dark" -Luke Smitherd </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Bazaar of Bad Dreams" -Stephen King </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "In the Barn" -Piers Anthony </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Spire" -William Golding </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Your Name is in the Book" -Luke Smitherd </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Breakthrough" -Ken Grimwood </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Neverwhere" -Neil Gaiman </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Heart of Darkness" -Joseph Conrad </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "To Kill a Mockingbird" -Harper Lee </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Chains" -Laurie Halse Anderson </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Go Set a Watchman" -Harper Lee </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Drums, Girls, &amp; Dangerous Pie" -Jordan Sonnenblick </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Dark Tales" -various authors </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Light Who Shines" -Lilo Abernathy </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Hold On Until Your Fingers Break" -Luke Smitherd </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Fountains of Paradise" -Arthur C. Clarke </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Last Question" -Isaac Asimov </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "August Heat" -W. F. Harvey </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Stone Man" -Luke Smitherd </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Finders Keepers" -Stephen King </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Stardust" -Neil Gaiman </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Dark Screams, Volume 1" -various authors- </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Ready Player One" -Ernest Cline </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Turn of the Screw" -Henry James </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Femme du Chaos" -Kristen Duval </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Moonstone" -Wilke Collins </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Gray Shadows" -Julia Gousseva </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Slan" -A.E. van Vogt </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Descant" -Piers Anthony </t>
-  </si>
-  <si>
     <t>5x readings]</t>
   </si>
   <si>
@@ -429,64 +69,424 @@
     <t>Notes</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Artemis Fowl:  The Last Guardian" -Eoin Colfer</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Artemis Fowl:  The Atlantis Complex" -Eoin Colfer </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Artemis Fowl:  The Time Paradox" -Eoin Colfer </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Collected Works of Philip K. Dick:  Volume 1- The King of the Elves" -Philip K. Dick</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Princess Bride: The 'Good Parts' Version" -William Goldman</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Skyrunner's Captain:  TalesFromElderland,Book2" -JD Mankowski </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Hiberverse:  Extinction Force" -David Mark Brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Ash Falls:  Inheritance" -Jeremy Schofield </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Traveling Vampire Show" -Richard Laymon </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Artemis Fowl:  The Lost Colony" -Eoin Colfer</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Agatha Christie:  An Autobiography" -Agatha Christie</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "How to Be a Vigilante:  A Diary" -Luke Smitherd</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Hiberverse:  Ranger's War" -David Mark Brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Theodore Boone:  Kid Lawyer" -John Grisham</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Firewall:  A Propagandist's Guide to Self-Defense" -Jack Nolan</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "William Shakespeare's Star Wars:  Verily A New Hope" -Ian Doescher </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2001:  A Space Odyssey" -Arthur C. Clarke</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "The Gunslinger Born:  A Graphic Novel" -Stephen King &amp; Robin Furth</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Necronomicon:  The Best Weird Tales" -H. P. Lovecraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Snapshot, 1988" -Joe Hill</t>
+    <t>"The Princess Bride: The 'Good Parts' Version" -William Goldman</t>
+  </si>
+  <si>
+    <t>“Lives of the Monster Dogs” -Kirsten Bakis</t>
+  </si>
+  <si>
+    <t>"Martian Time-Slip" -Philip K. Dick</t>
+  </si>
+  <si>
+    <t>"Lullaby" -Jonathan Maberry</t>
+  </si>
+  <si>
+    <t>"Elevation" &amp; "Laurie" -Stephen King</t>
+  </si>
+  <si>
+    <t>"The Switch House" -Tim Meyer</t>
+  </si>
+  <si>
+    <t>"Do Androids Dream of Electric Sheep" -Philip K. Dick</t>
+  </si>
+  <si>
+    <t>"Collected Works of Philip K. Dick: Volume 1- The King of the Elves" -Philip K. Dick</t>
+  </si>
+  <si>
+    <t>"Night" -Elie Wiesel</t>
+  </si>
+  <si>
+    <t>"Bumpy Night on the Walk of Fame" -Loretta Bolger Wish</t>
+  </si>
+  <si>
+    <t>"The Most Dangerous Game" Richard Connell</t>
+  </si>
+  <si>
+    <t>"Artemis Fowl: The Last Guardian" -Eoin Colfer</t>
+  </si>
+  <si>
+    <t>"Artemis Fowl: The Atlantis Complex" -Eoin Colfer</t>
+  </si>
+  <si>
+    <t>"Artemis Fowl: The Time Paradox" -Eoin Colfer</t>
+  </si>
+  <si>
+    <t>"The Cats of Cthulhu" -Chris W. Sears</t>
+  </si>
+  <si>
+    <t>"Tales of the Unusual" -Luke Smitherd</t>
+  </si>
+  <si>
+    <t>"Raiding Jotunheim- Valhalla Online, Book 2" -Kevin O. McLaughlin</t>
+  </si>
+  <si>
+    <t>"Valhalla Online" -Kevin O. McLaughlin</t>
+  </si>
+  <si>
+    <t>"The Picture of Dorian Gray" -Oscar Wilde</t>
+  </si>
+  <si>
+    <t>"Born on a Blue Day" -Daniel Temmet</t>
+  </si>
+  <si>
+    <t>"Space Opera" -Catherynne M. Valente</t>
+  </si>
+  <si>
+    <t>"The Outsider" -Stephen King</t>
+  </si>
+  <si>
+    <t>"Neuromancer" -William Gibson</t>
+  </si>
+  <si>
+    <t>"The Skyrunner's Captain: TalesFromElderland,Book2" -JD Mankowski</t>
+  </si>
+  <si>
+    <t>"A Long December" -Richard Chizmar</t>
+  </si>
+  <si>
+    <t>"The Moon is  Harsh Mistress" -Robert A. Heinlein</t>
+  </si>
+  <si>
+    <t>"Time for the Stars" -Robert A. Heinlein</t>
+  </si>
+  <si>
+    <t>"Man in the Empty Suit" -Sean Ferrell</t>
+  </si>
+  <si>
+    <t>"The Man Who Folded Himself" -David Gerrold</t>
+  </si>
+  <si>
+    <t>"Artemis" -Andy Weir</t>
+  </si>
+  <si>
+    <t>"The Martian" -Andy Weir</t>
+  </si>
+  <si>
+    <t>"Double Feature" -Owen King</t>
+  </si>
+  <si>
+    <t>"Widow's Point" -Richard Chizmar &amp; Billy Chizmar</t>
+  </si>
+  <si>
+    <t>"Sleeping Beauties" -Stephen King &amp; Owen King</t>
+  </si>
+  <si>
+    <t>"The Wendigo" -author unknown-</t>
+  </si>
+  <si>
+    <t>"The Secret of Chimneys" -Agatha Christie</t>
+  </si>
+  <si>
+    <t>"Greener Pastures" -Michael Wehunt</t>
+  </si>
+  <si>
+    <t>"The Christmas Spirit" -Brian James Freeman</t>
+  </si>
+  <si>
+    <t>"Hiberverse: Extinction Force" -David Mark Brown</t>
+  </si>
+  <si>
+    <t>"Ash Falls: Inheritance" -Jeremy Schofield</t>
+  </si>
+  <si>
+    <t>"Honey" -Sarah Sheldon</t>
+  </si>
+  <si>
+    <t>"Hex" -Thomas Olde Heuvelt</t>
+  </si>
+  <si>
+    <t>"The Nine Billion Names of God" -Arthur D. Clarke</t>
+  </si>
+  <si>
+    <t>"Drawing Dead" -Brian McKinley</t>
+  </si>
+  <si>
+    <t>"Chthon" -Piers Anthony</t>
+  </si>
+  <si>
+    <t>"Outlander" -Diana Gabaldon</t>
+  </si>
+  <si>
+    <t>"The Hitchhiker's Guide to the Galaxy" -Douglas Adams</t>
+  </si>
+  <si>
+    <t>"Gwendy's Button Box" -Stephen King &amp; Richard Chizmar</t>
+  </si>
+  <si>
+    <t>"Cemetery Dance, Issue #1" -various authors-</t>
+  </si>
+  <si>
+    <t>"The Hero with a Thousand Faces" -Joseph Campbell</t>
+  </si>
+  <si>
+    <t>"Mr. Bubbles and the Mystery of the Mayan Temple" -Chris Sears</t>
+  </si>
+  <si>
+    <t>"The Warlord of Mars" -Edgar Rice Burroughs</t>
+  </si>
+  <si>
+    <t>"The Gods of Mars" -Edgar Rice Burroughs</t>
+  </si>
+  <si>
+    <t>"The Wreck of the Titan" -Morgan Robertson</t>
+  </si>
+  <si>
+    <t>"A Princess of Mars" -Edgar Rice Burroughs</t>
+  </si>
+  <si>
+    <t>"Snapshot, 1988" -Joe Hill</t>
+  </si>
+  <si>
+    <t>"The Consciousness Plague" -Paul Levinson</t>
+  </si>
+  <si>
+    <t>"The Plot to Save Socrates" -Paul Levinson</t>
+  </si>
+  <si>
+    <t>"Urban Gothic" -Brian Keene</t>
+  </si>
+  <si>
+    <t>"The Consultant" -Bentley Little</t>
+  </si>
+  <si>
+    <t>"The Fireman" -Joe Hill</t>
+  </si>
+  <si>
+    <t>"The Marvels" -Brian Selznik</t>
+  </si>
+  <si>
+    <t>"Charlie the Choo-Choo" -Stephen King</t>
+  </si>
+  <si>
+    <t>"Last Rung on the Ladder" -David Martin</t>
+  </si>
+  <si>
+    <t>"The Traveling Vampire Show" -Richard Laymon</t>
+  </si>
+  <si>
+    <t>"Interview with the Vampire" -Anne Rice</t>
+  </si>
+  <si>
+    <t>"Limetown" -Zack Akers</t>
+  </si>
+  <si>
+    <t>"Artemis Fowl: The Lost Colony" -Eoin Colfer</t>
+  </si>
+  <si>
+    <t>"Cemetery Dance, Issue #73" -various authors-</t>
+  </si>
+  <si>
+    <t>"Hallowe'en Party" -Agatha Christie</t>
+  </si>
+  <si>
+    <t>"Five Little Pigs" -Agatha Christie</t>
+  </si>
+  <si>
+    <t>"Agatha Christie: An Autobiography" -Agatha Christie</t>
+  </si>
+  <si>
+    <t>"Save the Cat!" -Blake Snyder</t>
+  </si>
+  <si>
+    <t>"How to Be a Vigilante: A Diary" -Luke Smitherd</t>
+  </si>
+  <si>
+    <t>"The Brothers Karamazov" -Fyodor Dostoyevsky</t>
+  </si>
+  <si>
+    <t>"Eleven" -Patricia Reilly Giff</t>
+  </si>
+  <si>
+    <t>"What Dreams May Come" -Richard Matheson</t>
+  </si>
+  <si>
+    <t>"Inferno" -Dan Brown</t>
+  </si>
+  <si>
+    <t>"The Silver Scepter" -JD Mankowski</t>
+  </si>
+  <si>
+    <t>"The Halloween Tree" -Ray Bradbury</t>
+  </si>
+  <si>
+    <t>"The Halloween Man" -Douglas Clegg</t>
+  </si>
+  <si>
+    <t>"The Haunted" -Bentley Little</t>
+  </si>
+  <si>
+    <t>"Hiberverse: Ranger's War" -David Mark Brown</t>
+  </si>
+  <si>
+    <t>"The Thief of Always" -Clive Barker</t>
+  </si>
+  <si>
+    <t>"20th Century Ghosts" -Joe Hill</t>
+  </si>
+  <si>
+    <t>"End of Watch" -Stephen King</t>
+  </si>
+  <si>
+    <t>"The Long Walk" -Stephen King</t>
+  </si>
+  <si>
+    <t>"The Dispossessed" -Ursula K. Le Guin</t>
+  </si>
+  <si>
+    <t>"Dune" -Frank Herbert</t>
+  </si>
+  <si>
+    <t>"Armada" -Ernest Cline</t>
+  </si>
+  <si>
+    <t>"Patient Zero" -Jonathan Mayberry</t>
+  </si>
+  <si>
+    <t>"Son" -Lois Lowry</t>
+  </si>
+  <si>
+    <t>"The Adventures of Sherlock Holmes" -Arthur Conan Doyle</t>
+  </si>
+  <si>
+    <t>"Speaking From Among the Bones" -Alan Bradley</t>
+  </si>
+  <si>
+    <t>"City of Orphans" -Avi</t>
+  </si>
+  <si>
+    <t>"The Hound of the Baskervilles" -Arthur Conan Doyle</t>
+  </si>
+  <si>
+    <t>"The Physics of the Dead" -Luke Smitherd</t>
+  </si>
+  <si>
+    <t>"The Inquisitor's Apprentice" -Chris Moriarty</t>
+  </si>
+  <si>
+    <t>"Theodore Boone: Kid Lawyer" -John Grisham</t>
+  </si>
+  <si>
+    <t>"Firewall: A Propagandist's Guide to Self-Defense" -Jack Nolan</t>
+  </si>
+  <si>
+    <t>"Foundation" -Isaac Asimov</t>
+  </si>
+  <si>
+    <t>"Red Moon" -Benjamin Percy</t>
+  </si>
+  <si>
+    <t>"Outview" -Brandt Legg</t>
+  </si>
+  <si>
+    <t>"A Head Full of Knives" -Luke Smitherd</t>
+  </si>
+  <si>
+    <t>"In the Darkness" -Luke Smitherd</t>
+  </si>
+  <si>
+    <t>"Weird, Dark" -Luke Smitherd</t>
+  </si>
+  <si>
+    <t>"The Bazaar of Bad Dreams" -Stephen King</t>
+  </si>
+  <si>
+    <t>"In the Barn" -Piers Anthony</t>
+  </si>
+  <si>
+    <t>"The Spire" -William Golding</t>
+  </si>
+  <si>
+    <t>"Your Name is in the Book" -Luke Smitherd</t>
+  </si>
+  <si>
+    <t>"Breakthrough" -Ken Grimwood</t>
+  </si>
+  <si>
+    <t>"Neverwhere" -Neil Gaiman</t>
+  </si>
+  <si>
+    <t>"Heart of Darkness" -Joseph Conrad</t>
+  </si>
+  <si>
+    <t>"To Kill a Mockingbird" -Harper Lee</t>
+  </si>
+  <si>
+    <t>"Chains" -Laurie Halse Anderson</t>
+  </si>
+  <si>
+    <t>"Go Set a Watchman" -Harper Lee</t>
+  </si>
+  <si>
+    <t>"Drums, Girls, &amp; Dangerous Pie" -Jordan Sonnenblick</t>
+  </si>
+  <si>
+    <t>"Dark Tales" -various authors</t>
+  </si>
+  <si>
+    <t>"The Light Who Shines" -Lilo Abernathy</t>
+  </si>
+  <si>
+    <t>"Hold On Until Your Fingers Break" -Luke Smitherd</t>
+  </si>
+  <si>
+    <t>"The Fountains of Paradise" -Arthur C. Clarke</t>
+  </si>
+  <si>
+    <t>"William Shakespeare's Star Wars: Verily A New Hope" -Ian Doescher</t>
+  </si>
+  <si>
+    <t>"The Last Question" -Isaac Asimov</t>
+  </si>
+  <si>
+    <t>"2001: A Space Odyssey" -Arthur C. Clarke</t>
+  </si>
+  <si>
+    <t>"August Heat" -W. F. Harvey</t>
+  </si>
+  <si>
+    <t>"The Stone Man" -Luke Smitherd</t>
+  </si>
+  <si>
+    <t>"The Gunslinger Born: A Graphic Novel" -Stephen King &amp; Robin Furth</t>
+  </si>
+  <si>
+    <t>"Finders Keepers" -Stephen King</t>
+  </si>
+  <si>
+    <t>"Stardust" -Neil Gaiman</t>
+  </si>
+  <si>
+    <t>"Dark Screams, Volume 1" -various authors-</t>
+  </si>
+  <si>
+    <t>"Ready Player One" -Ernest Cline</t>
+  </si>
+  <si>
+    <t>"The Turn of the Screw" -Henry James</t>
+  </si>
+  <si>
+    <t>"Necronomicon: The Best Weird Tales" -H. P. Lovecraft</t>
+  </si>
+  <si>
+    <t>"Femme du Chaos" -Kristen Duval</t>
+  </si>
+  <si>
+    <t>"The Moonstone" -Wilke Collins</t>
+  </si>
+  <si>
+    <t>"Gray Shadows" -Julia Gousseva</t>
+  </si>
+  <si>
+    <t>"Slan" -A.E. van Vogt</t>
+  </si>
+  <si>
+    <t>"Descant" -Piers Anthony</t>
+  </si>
+  <si>
+    <t>"Head On" -John Scalzi</t>
+  </si>
+  <si>
+    <t>"Lock In" -John Scalzi</t>
   </si>
 </sst>
 </file>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -855,16 +855,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>134</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>135</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>136</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15">
@@ -872,10 +872,10 @@
         <v>43465</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15">
@@ -883,10 +883,10 @@
         <v>43458</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15">
@@ -894,10 +894,10 @@
         <v>43429</v>
       </c>
       <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15">
@@ -905,10 +905,10 @@
         <v>43428</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>17</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15">
@@ -916,10 +916,10 @@
         <v>43422</v>
       </c>
       <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15">
@@ -927,10 +927,10 @@
         <v>43416</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15">
@@ -938,10 +938,10 @@
         <v>43409</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15">
@@ -949,10 +949,10 @@
         <v>43387</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>24</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15">
@@ -960,10 +960,10 @@
         <v>43352</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15">
@@ -971,10 +971,10 @@
         <v>43337</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15">
@@ -982,10 +982,10 @@
         <v>43334</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
@@ -996,10 +996,10 @@
         <v>43326</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>28</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15">
@@ -1007,10 +1007,10 @@
         <v>43313</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>29</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15">
@@ -1018,10 +1018,10 @@
         <v>43311</v>
       </c>
       <c r="B15" t="s">
-        <v>139</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15">
@@ -1029,10 +1029,10 @@
         <v>43300</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15">
@@ -1040,10 +1040,10 @@
         <v>43295</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15">
@@ -1051,10 +1051,10 @@
         <v>43294</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15">
@@ -1062,10 +1062,10 @@
         <v>43292</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15">
@@ -1073,10 +1073,10 @@
         <v>43290</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15">
@@ -1084,10 +1084,10 @@
         <v>43286</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15">
@@ -1095,10 +1095,10 @@
         <v>43285</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>155</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15">
@@ -1106,10 +1106,10 @@
         <v>43284</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>156</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15">
@@ -1117,10 +1117,10 @@
         <v>43282</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15">
@@ -1128,10 +1128,10 @@
         <v>43267</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15">
@@ -1139,10 +1139,10 @@
         <v>43254</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15">
@@ -1150,10 +1150,10 @@
         <v>43243</v>
       </c>
       <c r="B27" t="s">
-        <v>142</v>
+        <v>40</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15">
@@ -1161,10 +1161,10 @@
         <v>43235</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15">
@@ -1172,10 +1172,10 @@
         <v>43208</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15">
@@ -1183,10 +1183,10 @@
         <v>43187</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15">
@@ -1194,10 +1194,10 @@
         <v>43178</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15">
@@ -1205,10 +1205,10 @@
         <v>43153</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15">
@@ -1216,10 +1216,10 @@
         <v>43137</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15">
@@ -1227,10 +1227,10 @@
         <v>43146</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15">
@@ -1238,10 +1238,10 @@
         <v>43117</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15">
@@ -1249,10 +1249,10 @@
         <v>43114</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15">
@@ -1260,10 +1260,10 @@
         <v>43076</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15">
@@ -1271,10 +1271,10 @@
         <v>43037</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
         <v>0</v>
@@ -1285,10 +1285,10 @@
         <v>43010</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15">
@@ -1296,10 +1296,10 @@
         <v>42997</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15">
@@ -1307,10 +1307,10 @@
         <v>42978</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
       <c r="D41" t="s">
         <v>1</v>
@@ -1321,10 +1321,10 @@
         <v>42976</v>
       </c>
       <c r="B42" t="s">
-        <v>143</v>
+        <v>55</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15">
@@ -1332,10 +1332,10 @@
         <v>42963</v>
       </c>
       <c r="B43" t="s">
-        <v>144</v>
+        <v>56</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15">
@@ -1343,10 +1343,10 @@
         <v>42954</v>
       </c>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
         <v>2</v>
@@ -1357,10 +1357,10 @@
         <v>42948</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15">
@@ -1368,10 +1368,10 @@
         <v>42944</v>
       </c>
       <c r="B46" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
       <c r="D46" t="s">
         <v>0</v>
@@ -1382,10 +1382,10 @@
         <v>42915</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15">
@@ -1393,10 +1393,10 @@
         <v>42905</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15">
@@ -1404,13 +1404,13 @@
         <v>42903</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15">
@@ -1418,10 +1418,10 @@
         <v>42896</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15">
@@ -1429,10 +1429,10 @@
         <v>42873</v>
       </c>
       <c r="B51" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15">
@@ -1440,10 +1440,10 @@
         <v>42872</v>
       </c>
       <c r="B52" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15">
@@ -1451,10 +1451,10 @@
         <v>42865</v>
       </c>
       <c r="B53" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>130</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15">
@@ -1462,10 +1462,10 @@
         <v>42861</v>
       </c>
       <c r="B54" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15">
@@ -1473,10 +1473,10 @@
         <v>42852</v>
       </c>
       <c r="B55" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15">
@@ -1484,10 +1484,10 @@
         <v>42842</v>
       </c>
       <c r="B56" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15">
@@ -1495,10 +1495,10 @@
         <v>42834</v>
       </c>
       <c r="B57" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
       <c r="D57" t="s">
         <v>0</v>
@@ -1509,10 +1509,10 @@
         <v>42834</v>
       </c>
       <c r="B58" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15">
@@ -1520,10 +1520,10 @@
         <v>42805</v>
       </c>
       <c r="B59" t="s">
-        <v>156</v>
+        <v>72</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
       <c r="D59" t="s">
         <v>0</v>
@@ -1534,10 +1534,10 @@
         <v>42798</v>
       </c>
       <c r="B60" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
       <c r="D60" t="s">
         <v>0</v>
@@ -1548,10 +1548,10 @@
         <v>42798</v>
       </c>
       <c r="B61" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15">
@@ -1559,10 +1559,10 @@
         <v>42790</v>
       </c>
       <c r="B62" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>130</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15">
@@ -1570,10 +1570,10 @@
         <v>42778</v>
       </c>
       <c r="B63" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>131</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15">
@@ -1581,10 +1581,10 @@
         <v>27785</v>
       </c>
       <c r="B64" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15">
@@ -1592,10 +1592,10 @@
         <v>42746</v>
       </c>
       <c r="B65" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15">
@@ -1603,10 +1603,10 @@
         <v>42735</v>
       </c>
       <c r="B66" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="D66" t="s">
         <v>2</v>
@@ -1617,10 +1617,10 @@
         <v>42733</v>
       </c>
       <c r="B67" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15">
@@ -1628,10 +1628,10 @@
         <v>42710</v>
       </c>
       <c r="B68" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>132</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15">
@@ -1639,10 +1639,10 @@
         <v>42699</v>
       </c>
       <c r="B69" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15">
@@ -1650,10 +1650,10 @@
         <v>42677</v>
       </c>
       <c r="B70" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15">
@@ -1661,10 +1661,10 @@
         <v>42674</v>
       </c>
       <c r="B71" t="s">
-        <v>146</v>
+        <v>84</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15">
@@ -1672,10 +1672,10 @@
         <v>42659</v>
       </c>
       <c r="B72" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15">
@@ -1683,10 +1683,10 @@
         <v>42657</v>
       </c>
       <c r="B73" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15">
@@ -1694,10 +1694,10 @@
         <v>42649</v>
       </c>
       <c r="B74" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15">
@@ -1705,10 +1705,10 @@
         <v>42641</v>
       </c>
       <c r="B75" t="s">
-        <v>147</v>
+        <v>88</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15">
@@ -1716,10 +1716,10 @@
         <v>42640</v>
       </c>
       <c r="B76" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15">
@@ -1727,10 +1727,10 @@
         <v>42638</v>
       </c>
       <c r="B77" t="s">
-        <v>148</v>
+        <v>90</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15">
@@ -1738,10 +1738,10 @@
         <v>42633</v>
       </c>
       <c r="B78" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>131</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15">
@@ -1749,10 +1749,10 @@
         <v>42626</v>
       </c>
       <c r="B79" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15">
@@ -1760,10 +1760,10 @@
         <v>42616</v>
       </c>
       <c r="B80" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15">
@@ -1771,10 +1771,10 @@
         <v>42613</v>
       </c>
       <c r="B81" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="15">
@@ -1782,10 +1782,10 @@
         <v>42604</v>
       </c>
       <c r="B82" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="15">
@@ -1793,10 +1793,10 @@
         <v>42601</v>
       </c>
       <c r="B83" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>130</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15">
@@ -1804,10 +1804,10 @@
         <v>42599</v>
       </c>
       <c r="B84" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="15">
@@ -1815,10 +1815,10 @@
         <v>42596</v>
       </c>
       <c r="B85" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15">
@@ -1826,10 +1826,10 @@
         <v>42583</v>
       </c>
       <c r="B86" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15">
@@ -1837,10 +1837,10 @@
         <v>42581</v>
       </c>
       <c r="B87" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15">
@@ -1848,10 +1848,10 @@
         <v>42579</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15">
@@ -1859,10 +1859,10 @@
         <v>42571</v>
       </c>
       <c r="B89" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="15">
@@ -1870,10 +1870,10 @@
         <v>42562</v>
       </c>
       <c r="B90" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="15">
@@ -1881,10 +1881,10 @@
         <v>42559</v>
       </c>
       <c r="B91" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15">
@@ -1892,10 +1892,10 @@
         <v>42548</v>
       </c>
       <c r="B92" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="15">
@@ -1903,10 +1903,10 @@
         <v>42525</v>
       </c>
       <c r="B93" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>130</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15">
@@ -1914,10 +1914,10 @@
         <v>42522</v>
       </c>
       <c r="B94" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="15">
@@ -1925,10 +1925,10 @@
         <v>42506</v>
       </c>
       <c r="B95" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="15">
@@ -1936,10 +1936,10 @@
         <v>42494</v>
       </c>
       <c r="B96" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15">
@@ -1947,10 +1947,10 @@
         <v>42479</v>
       </c>
       <c r="B97" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15">
@@ -1958,10 +1958,10 @@
         <v>42464</v>
       </c>
       <c r="B98" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15">
@@ -1969,10 +1969,10 @@
         <v>42464</v>
       </c>
       <c r="B99" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15">
@@ -1980,10 +1980,10 @@
         <v>42458</v>
       </c>
       <c r="B100" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15">
@@ -1991,10 +1991,10 @@
         <v>42458</v>
       </c>
       <c r="B101" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15">
@@ -2002,10 +2002,10 @@
         <v>42457</v>
       </c>
       <c r="B102" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>132</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15">
@@ -2013,10 +2013,10 @@
         <v>42445</v>
       </c>
       <c r="B103" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15">
@@ -2024,10 +2024,10 @@
         <v>42442</v>
       </c>
       <c r="B104" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15">
@@ -2035,10 +2035,10 @@
         <v>42432</v>
       </c>
       <c r="B105" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15">
@@ -2046,10 +2046,10 @@
         <v>42430</v>
       </c>
       <c r="B106" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>130</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15">
@@ -2057,10 +2057,10 @@
         <v>42395</v>
       </c>
       <c r="B107" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15">
@@ -2068,10 +2068,10 @@
         <v>42382</v>
       </c>
       <c r="B108" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15">
@@ -2079,10 +2079,10 @@
         <v>42366</v>
       </c>
       <c r="B109" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15">
@@ -2090,10 +2090,10 @@
         <v>42348</v>
       </c>
       <c r="B110" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15">
@@ -2101,10 +2101,10 @@
         <v>42330</v>
       </c>
       <c r="B111" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
       <c r="D111" t="s">
         <v>1</v>
@@ -2115,10 +2115,10 @@
         <v>42317</v>
       </c>
       <c r="B112" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>132</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15">
@@ -2126,10 +2126,10 @@
         <v>42314</v>
       </c>
       <c r="B113" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>130</v>
+        <v>10</v>
       </c>
       <c r="D113" t="s">
         <v>0</v>
@@ -2140,10 +2140,10 @@
         <v>42305</v>
       </c>
       <c r="B114" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15">
@@ -2151,10 +2151,10 @@
         <v>42296</v>
       </c>
       <c r="B115" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15">
@@ -2162,10 +2162,10 @@
         <v>42273</v>
       </c>
       <c r="B116" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>132</v>
+        <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15">
@@ -2173,10 +2173,10 @@
         <v>42267</v>
       </c>
       <c r="B117" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15">
@@ -2184,10 +2184,10 @@
         <v>42254</v>
       </c>
       <c r="B118" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15">
@@ -2195,10 +2195,10 @@
         <v>42252</v>
       </c>
       <c r="B119" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15">
@@ -2206,10 +2206,10 @@
         <v>42251</v>
       </c>
       <c r="B120" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15">
@@ -2217,10 +2217,10 @@
         <v>42245</v>
       </c>
       <c r="B121" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15">
@@ -2228,10 +2228,10 @@
         <v>42239</v>
       </c>
       <c r="B122" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15">
@@ -2239,10 +2239,10 @@
         <v>42231</v>
       </c>
       <c r="B123" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15">
@@ -2250,10 +2250,10 @@
         <v>42213</v>
       </c>
       <c r="B124" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15">
@@ -2261,10 +2261,10 @@
         <v>42197</v>
       </c>
       <c r="B125" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>130</v>
+        <v>10</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15">
@@ -2272,10 +2272,10 @@
         <v>42193</v>
       </c>
       <c r="B126" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
       <c r="D126" t="s">
         <v>1</v>
@@ -2286,10 +2286,10 @@
         <v>42192</v>
       </c>
       <c r="B127" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15">
@@ -2297,10 +2297,10 @@
         <v>42161</v>
       </c>
       <c r="B128" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
       <c r="D128" t="s">
         <v>0</v>
@@ -2311,10 +2311,10 @@
         <v>42164</v>
       </c>
       <c r="B129" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="15">
@@ -2322,10 +2322,10 @@
         <v>42173</v>
       </c>
       <c r="B130" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="15">
@@ -2333,10 +2333,10 @@
         <v>42178</v>
       </c>
       <c r="B131" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="15">
@@ -2344,10 +2344,10 @@
         <v>42184</v>
       </c>
       <c r="B132" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="15">
@@ -2355,10 +2355,10 @@
         <v>42150</v>
       </c>
       <c r="B133" t="s">
-        <v>115</v>
+        <v>146</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="15">
@@ -2366,10 +2366,10 @@
         <v>42145</v>
       </c>
       <c r="B134" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="15">
@@ -2377,10 +2377,10 @@
         <v>42138</v>
       </c>
       <c r="B135" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="15">
@@ -2388,10 +2388,10 @@
         <v>42124</v>
       </c>
       <c r="B136" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="15">
@@ -2399,10 +2399,10 @@
         <v>42089</v>
       </c>
       <c r="B137" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="15">
@@ -2410,10 +2410,10 @@
         <v>42084</v>
       </c>
       <c r="B138" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>130</v>
+        <v>10</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="15">
@@ -2421,10 +2421,10 @@
         <v>42019</v>
       </c>
       <c r="B139" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>131</v>
+        <v>11</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="15">
@@ -2432,10 +2432,10 @@
         <v>42010</v>
       </c>
       <c r="B140" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>130</v>
+        <v>10</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="15">
@@ -2443,10 +2443,10 @@
         <v>42008</v>
       </c>
       <c r="B141" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>